<commit_message>
Modify the Wishing Wall quest
</commit_message>
<xml_diff>
--- a/src/main/resources/许愿墙.xlsx
+++ b/src/main/resources/许愿墙.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28526"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24026"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\desktop\get_jobs\src\main\resources\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\get_jobs\src\main\resources\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9AB1FEA4-1826-43B6-AA8B-F3FCC3C378BC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A8C68E06-1371-4496-A73E-E24FCFEF613E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-28920" yWindow="2205" windowWidth="29040" windowHeight="15720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-110" yWindow="-110" windowWidth="25820" windowHeight="15500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="6" uniqueCount="6">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="8" uniqueCount="7">
   <si>
     <t>你想找什么样的工作？</t>
   </si>
@@ -44,24 +44,35 @@
   <si>
     <t>逆向开发</t>
   </si>
+  <si>
+    <t>Java+AI</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="2" x14ac:knownFonts="1">
+  <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="10"/>
       <color theme="1"/>
-      <name val="Calibri"/>
+      <name val="等线"/>
       <family val="2"/>
       <scheme val="minor"/>
     </font>
     <font>
       <sz val="9.75"/>
       <color rgb="FF000000"/>
-      <name val="Calibri"/>
+      <name val="等线"/>
       <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="9"/>
+      <name val="等线"/>
+      <family val="3"/>
+      <charset val="134"/>
       <scheme val="minor"/>
     </font>
   </fonts>
@@ -158,9 +169,9 @@
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office 2013 - 2022 主题">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office 主题​​">
   <a:themeElements>
-    <a:clrScheme name="Office 2013 - 2022">
+    <a:clrScheme name="Office">
       <a:dk1>
         <a:sysClr val="windowText" lastClr="000000"/>
       </a:dk1>
@@ -198,7 +209,7 @@
         <a:srgbClr val="954F72"/>
       </a:folHlink>
     </a:clrScheme>
-    <a:fontScheme name="Office 2013 - 2022">
+    <a:fontScheme name="Office">
       <a:majorFont>
         <a:latin typeface="Calibri Light" panose="020F0302020204030204"/>
         <a:ea typeface=""/>
@@ -304,7 +315,7 @@
         <a:font script="Tfng" typeface="Ebrima"/>
       </a:minorFont>
     </a:fontScheme>
-    <a:fmtScheme name="Office 2013 - 2022">
+    <a:fmtScheme name="Office">
       <a:fillStyleLst>
         <a:solidFill>
           <a:schemeClr val="phClr"/>
@@ -446,7 +457,7 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office 2013 - 2022 Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
@@ -460,7 +471,7 @@
   <dimension ref="A1:T200"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A3" sqref="A3"/>
+      <selection activeCell="G10" sqref="G10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14" defaultRowHeight="13" x14ac:dyDescent="0.3"/>
@@ -548,8 +559,12 @@
       <c r="T3" s="1"/>
     </row>
     <row r="4" spans="1:20" x14ac:dyDescent="0.3">
-      <c r="A4" s="2"/>
-      <c r="B4" s="2"/>
+      <c r="A4" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="B4" s="2" t="s">
+        <v>4</v>
+      </c>
       <c r="C4" s="1"/>
       <c r="D4" s="1"/>
       <c r="E4" s="1"/>
@@ -4882,6 +4897,8 @@
       <c r="T200" s="1"/>
     </row>
   </sheetData>
+  <phoneticPr fontId="2" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="1200" verticalDpi="1200" r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
Updated the content of the wishing wall
</commit_message>
<xml_diff>
--- a/src/main/resources/许愿墙.xlsx
+++ b/src/main/resources/许愿墙.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28526"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24026"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\desktop\get_jobs\src\main\resources\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\get_jobs\src\main\resources\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9AB1FEA4-1826-43B6-AA8B-F3FCC3C378BC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C86BDA26-A1C1-4308-948A-A1CB9B26FFF8}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-28920" yWindow="2205" windowWidth="29040" windowHeight="15720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-110" yWindow="-110" windowWidth="25820" windowHeight="15500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="6" uniqueCount="6">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="8" uniqueCount="7">
   <si>
     <t>你想找什么样的工作？</t>
   </si>
@@ -44,24 +44,35 @@
   <si>
     <t>逆向开发</t>
   </si>
+  <si>
+    <t>Java+AI</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="2" x14ac:knownFonts="1">
+  <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="10"/>
       <color theme="1"/>
-      <name val="Calibri"/>
+      <name val="等线"/>
       <family val="2"/>
       <scheme val="minor"/>
     </font>
     <font>
       <sz val="9.75"/>
       <color rgb="FF000000"/>
-      <name val="Calibri"/>
+      <name val="等线"/>
       <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="9"/>
+      <name val="等线"/>
+      <family val="3"/>
+      <charset val="134"/>
       <scheme val="minor"/>
     </font>
   </fonts>
@@ -158,9 +169,9 @@
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office 2013 - 2022 主题">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office 主题​​">
   <a:themeElements>
-    <a:clrScheme name="Office 2013 - 2022">
+    <a:clrScheme name="Office">
       <a:dk1>
         <a:sysClr val="windowText" lastClr="000000"/>
       </a:dk1>
@@ -198,7 +209,7 @@
         <a:srgbClr val="954F72"/>
       </a:folHlink>
     </a:clrScheme>
-    <a:fontScheme name="Office 2013 - 2022">
+    <a:fontScheme name="Office">
       <a:majorFont>
         <a:latin typeface="Calibri Light" panose="020F0302020204030204"/>
         <a:ea typeface=""/>
@@ -304,7 +315,7 @@
         <a:font script="Tfng" typeface="Ebrima"/>
       </a:minorFont>
     </a:fontScheme>
-    <a:fmtScheme name="Office 2013 - 2022">
+    <a:fmtScheme name="Office">
       <a:fillStyleLst>
         <a:solidFill>
           <a:schemeClr val="phClr"/>
@@ -446,7 +457,7 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office 2013 - 2022 Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
@@ -460,7 +471,7 @@
   <dimension ref="A1:T200"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A3" sqref="A3"/>
+      <selection activeCell="E5" sqref="E5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14" defaultRowHeight="13" x14ac:dyDescent="0.3"/>
@@ -548,8 +559,12 @@
       <c r="T3" s="1"/>
     </row>
     <row r="4" spans="1:20" x14ac:dyDescent="0.3">
-      <c r="A4" s="2"/>
-      <c r="B4" s="2"/>
+      <c r="A4" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="B4" s="2" t="s">
+        <v>4</v>
+      </c>
       <c r="C4" s="1"/>
       <c r="D4" s="1"/>
       <c r="E4" s="1"/>
@@ -4882,6 +4897,8 @@
       <c r="T200" s="1"/>
     </row>
   </sheetData>
+  <phoneticPr fontId="2" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="1200" verticalDpi="1200" r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>